<commit_message>
Update Basler Test on a2A1920
</commit_message>
<xml_diff>
--- a/tests/test_25_10.xlsx
+++ b/tests/test_25_10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_git\lense-ressources\lensecam\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tools\git_repo\LEnsE\ressources\lensecam\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F651439-C362-4864-A2FB-CCF1E71C9AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2DEDBF-CF6B-4FED-9EDB-532AB5C1BAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="2745" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Obscurité" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Mean 1</t>
   </si>
@@ -109,10 +109,13 @@
     <t>Std1^2</t>
   </si>
   <si>
-    <t>Mean 1-m0</t>
+    <t>Mean2-m0</t>
   </si>
   <si>
-    <t>Mean2-m0</t>
+    <t>u-udark (DN)</t>
+  </si>
+  <si>
+    <t>Sig^2-Sigd^2 (DN^2)</t>
   </si>
 </sst>
 </file>
@@ -1268,6 +1271,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Dark signal (DN) fct</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> Integration Time (us)</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2283,6 +2316,385 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sig^2-Sigd^2 (DN^2) / u-Udark</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (DN)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Flux!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sig^2-Sigd^2 (DN^2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Flux!$C$5:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>552</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1389</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2230</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3065</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3587</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3758</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4012</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Flux!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.28090000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62.0944</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>175.82759999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>303.45640000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>501.31210000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>705.43359999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>744.7441</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1524.1215999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DA61-49D3-911A-B20493D32B9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1923993647"/>
+        <c:axId val="1923994127"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1923993647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1923994127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1923994127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1923993647"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2323,17 +2735,17 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Flux!$J$4</c:f>
+              <c:f>Flux!$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Std1^2</c:v>
+                  <c:v>Sig^2-Sigd^2 (DN^2)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2400,66 +2812,42 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Flux!$J$5:$J$12</c:f>
+              <c:f>Flux!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.27040000000000003</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.360000000000003</c:v>
+                  <c:v>590</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>1427</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82.809999999999988</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>119.68359999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>159.01209999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>183.87360000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>239.32090000000002</c:v>
+                  <c:v>2268</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Flux!$H$5:$H$12</c:f>
+              <c:f>Flux!$E$5:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.28090000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>175</c:v>
+                  <c:v>62.0944</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>439</c:v>
+                  <c:v>175.82759999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>705</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>972</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1236</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1414</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1772</c:v>
+                  <c:v>303.45640000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2467,7 +2855,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1E38-4A33-8521-84AE3B638B18}"/>
+              <c16:uniqueId val="{00000000-F211-4EE1-B193-6AD55643B9B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2479,11 +2867,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="726825040"/>
-        <c:axId val="726827440"/>
+        <c:axId val="1473825455"/>
+        <c:axId val="1473825935"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="726825040"/>
+        <c:axId val="1473825455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2540,12 +2928,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="726827440"/>
+        <c:crossAx val="1473825935"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="726827440"/>
+        <c:axId val="1473825935"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2602,7 +2990,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="726825040"/>
+        <c:crossAx val="1473825455"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2658,7 +3046,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -3405,6 +3793,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5470,6 +5898,526 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5985,7 +6933,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6578,15 +7526,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:colOff>171449</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6654,23 +7602,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Graphique 4">
+        <xdr:cNvPr id="2" name="Graphique 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9BA255A-2DD2-F397-682B-5271FD6D88EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C24CF8B-B850-43FE-ACBD-2F94C1D7E4D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6683,6 +7631,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97613654-9C89-9040-34E2-668C66EF652D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6998,7 +7982,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E2"/>
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7709,8 +8693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" activeCellId="1" sqref="B4:B8 E4:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7746,19 +8730,19 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s">
         <v>5</v>

</xml_diff>